<commit_message>
Emit header on data event.
</commit_message>
<xml_diff>
--- a/tests/assets/with-header.xlsx
+++ b/tests/assets/with-header.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79913FD1-E024-4200-A6FD-44C28FA25CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8119C74-788F-4F18-A28D-9E819D5FC5AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>hello</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>column2</t>
+  </si>
+  <si>
+    <t>column3</t>
   </si>
 </sst>
 </file>
@@ -347,27 +350,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>123.123</v>
       </c>
     </row>

</xml_diff>